<commit_message>
verified the string and compare to get the id of foreign key
</commit_message>
<xml_diff>
--- a/wwwroot/uploads/book.xlsx
+++ b/wwwroot/uploads/book.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\c#-projects\asp-dotnet\sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE6E6C43-9C2D-4A47-8979-686549F724FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4374F45-3E87-4CB0-BA26-7E6E39F93279}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1884" yWindow="1884" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,30 +25,39 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t xml:space="preserve">Where we go </t>
-  </si>
-  <si>
-    <t>This book is about universe</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
   <si>
     <t>Sherwin</t>
   </si>
   <si>
-    <t>image</t>
-  </si>
-  <si>
-    <t>Python</t>
-  </si>
-  <si>
-    <t>Python tutorial</t>
-  </si>
-  <si>
     <t>Paika</t>
   </si>
   <si>
     <t>image2</t>
+  </si>
+  <si>
+    <t>Programming</t>
+  </si>
+  <si>
+    <t>Asp.NetCore</t>
+  </si>
+  <si>
+    <t>This book is about programming</t>
+  </si>
+  <si>
+    <t>image1</t>
+  </si>
+  <si>
+    <t>Universe</t>
+  </si>
+  <si>
+    <t>Universe1</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>image3</t>
   </si>
 </sst>
 </file>
@@ -366,58 +375,81 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C1">
         <v>99</v>
       </c>
-      <c r="D1">
-        <v>5</v>
+      <c r="D1" t="s">
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F1">
         <v>1000</v>
       </c>
       <c r="G1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C2">
         <v>199</v>
       </c>
-      <c r="D2">
-        <v>2</v>
+      <c r="D2" t="s">
+        <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="F2">
         <v>2000</v>
       </c>
       <c r="G2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
         <v>7</v>
+      </c>
+      <c r="C3">
+        <v>199</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>2000</v>
+      </c>
+      <c r="G3" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>